<commit_message>
Update docs and site.
</commit_message>
<xml_diff>
--- a/docs/reference/figures/packages_tables.xlsx
+++ b/docs/reference/figures/packages_tables.xlsx
@@ -31,6 +31,102 @@
     <author>Jonas Kristoffer Lindeløv</author>
   </authors>
   <commentList>
+    <comment ref="L2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonas Kristoffer Lindeløv:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Autoregression for time-series</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonas Kristoffer Lindeløv:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Can parameters be shared between segments or across levels?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonas Kristoffer Lindeløv:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Per segment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonas Kristoffer Lindeløv:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Per segment</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -60,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="80">
   <si>
     <t>ecp</t>
   </si>
@@ -138,9 +234,6 @@
   </si>
   <si>
     <t>auto: int</t>
-  </si>
-  <si>
-    <t>specify: slope + int</t>
   </si>
   <si>
     <t>specify: slope</t>
@@ -347,7 +440,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,12 +462,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -542,9 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -572,29 +656,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,13 +968,13 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="38" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
@@ -912,92 +993,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>65</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>73</v>
-      </c>
       <c r="M2" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>34</v>
+      <c r="B3" s="31" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="14" t="s">
@@ -1009,7 +1090,7 @@
       <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="L3" s="33" t="s">
         <v>11</v>
       </c>
       <c r="M3" s="14" t="s">
@@ -1020,25 +1101,25 @@
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>27</v>
+      <c r="C4" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1050,7 +1131,7 @@
       <c r="K4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="17" t="s">
@@ -1061,25 +1142,25 @@
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>61</v>
+      <c r="E5" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="G5" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="14" t="s">
@@ -1091,7 +1172,7 @@
       <c r="K5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="17" t="s">
@@ -1102,7 +1183,7 @@
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -1117,10 +1198,10 @@
       <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="27" t="s">
+      <c r="G6" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -1132,7 +1213,7 @@
       <c r="K6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M6" s="17" t="s">
@@ -1143,7 +1224,7 @@
       <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1158,10 +1239,10 @@
       <c r="F7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="27" t="s">
+      <c r="G7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="14" t="s">
@@ -1173,7 +1254,7 @@
       <c r="K7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="L7" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M7" s="17" t="s">
@@ -1182,13 +1263,13 @@
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>51</v>
-      </c>
       <c r="C8" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
@@ -1199,10 +1280,10 @@
       <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="14" t="s">
@@ -1211,10 +1292,10 @@
       <c r="J8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="33" t="s">
+      <c r="K8" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="17" t="s">
@@ -1225,11 +1306,11 @@
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>10</v>
@@ -1240,11 +1321,11 @@
       <c r="F9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>35</v>
+      <c r="G9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>34</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>11</v>
@@ -1255,7 +1336,7 @@
       <c r="K9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="17" t="s">
@@ -1266,11 +1347,11 @@
       <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -1281,10 +1362,10 @@
       <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="27" t="s">
+      <c r="G10" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="14" t="s">
@@ -1296,7 +1377,7 @@
       <c r="K10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="17" t="s">
@@ -1305,16 +1386,16 @@
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>41</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>10</v>
@@ -1322,10 +1403,10 @@
       <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="G11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="14" t="s">
@@ -1337,7 +1418,7 @@
       <c r="K11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="L11" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="15" t="s">
@@ -1346,27 +1427,27 @@
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="C12" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="D12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="14" t="s">
@@ -1378,7 +1459,7 @@
       <c r="K12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="L12" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="15" t="s">
@@ -1387,13 +1468,13 @@
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>53</v>
-      </c>
       <c r="C13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
@@ -1404,10 +1485,10 @@
       <c r="F13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="14" t="s">
@@ -1419,7 +1500,7 @@
       <c r="K13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="32" t="s">
         <v>10</v>
       </c>
       <c r="M13" s="15" t="s">
@@ -1520,54 +1601,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="20" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>33</v>
+      <c r="G2" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="K2" s="21"/>
     </row>
@@ -1575,8 +1656,8 @@
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>34</v>
+      <c r="B3" s="31" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>11</v>
@@ -1590,7 +1671,7 @@
       <c r="F3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="14" t="s">
@@ -1600,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -1608,7 +1689,7 @@
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -1623,17 +1704,17 @@
       <c r="F4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K4" s="23"/>
     </row>
@@ -1641,7 +1722,7 @@
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -1656,7 +1737,7 @@
       <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="17" t="s">
@@ -1674,7 +1755,7 @@
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1689,7 +1770,7 @@
       <c r="F6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="17" t="s">
@@ -1707,7 +1788,7 @@
       <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -1722,7 +1803,7 @@
       <c r="F7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -1738,11 +1819,11 @@
     </row>
     <row r="8" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>51</v>
-      </c>
       <c r="C8" s="17" t="s">
         <v>10</v>
       </c>
@@ -1755,7 +1836,7 @@
       <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="17" t="s">
@@ -1773,7 +1854,7 @@
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -1788,7 +1869,7 @@
       <c r="F9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="17" t="s">
@@ -1806,7 +1887,7 @@
       <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -1821,7 +1902,7 @@
       <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="17" t="s">
@@ -1837,9 +1918,9 @@
     </row>
     <row r="11" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="33"/>
+        <v>39</v>
+      </c>
+      <c r="B11" s="32"/>
       <c r="C11" s="17" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1933,7 @@
       <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="17" t="s">
@@ -1868,11 +1949,11 @@
     </row>
     <row r="12" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>48</v>
-      </c>
       <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1966,7 @@
       <c r="F12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="17" t="s">
@@ -1895,17 +1976,17 @@
         <v>10</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>53</v>
-      </c>
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1999,7 @@
       <c r="F13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="17" t="s">
@@ -2005,39 +2086,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="F2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -2047,8 +2128,8 @@
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>34</v>
+      <c r="B3" s="37" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>11</v>
@@ -2059,8 +2140,8 @@
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>77</v>
+      <c r="F3" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>11</v>
@@ -2073,7 +2154,7 @@
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2086,7 +2167,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>10</v>
@@ -2099,7 +2180,7 @@
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="37" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -2112,7 +2193,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>10</v>
@@ -2125,7 +2206,7 @@
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="37" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -2138,10 +2219,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>61</v>
+        <v>75</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>60</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2151,7 +2232,7 @@
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -2164,7 +2245,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>10</v>
@@ -2175,11 +2256,11 @@
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>51</v>
-      </c>
       <c r="C8" s="11" t="s">
         <v>10</v>
       </c>
@@ -2190,7 +2271,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>10</v>
@@ -2203,7 +2284,7 @@
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="37" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -2216,7 +2297,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>10</v>
@@ -2229,7 +2310,7 @@
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -2242,7 +2323,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>10</v>
@@ -2253,11 +2334,11 @@
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>41</v>
-      </c>
       <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2349,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>10</v>
@@ -2279,11 +2360,11 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>48</v>
-      </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
@@ -2294,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>10</v>
@@ -2305,11 +2386,11 @@
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>53</v>
-      </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
@@ -2320,7 +2401,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Ready for CRAN resubmission
</commit_message>
<xml_diff>
--- a/docs/reference/figures/packages_tables.xlsx
+++ b/docs/reference/figures/packages_tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35085" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35085"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -445,9 +445,6 @@
     <t>auto: slope + int</t>
   </si>
   <si>
-    <t>auto: int</t>
-  </si>
-  <si>
     <t>specify: slope</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>2.0.0</t>
   </si>
   <si>
-    <t>auto: int?</t>
-  </si>
-  <si>
     <t>AIC and deviance</t>
   </si>
   <si>
@@ -547,9 +541,6 @@
     <t>AR(N)</t>
   </si>
   <si>
-    <t>AR(2)</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -617,6 +608,15 @@
   </si>
   <si>
     <t>hyper</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int?</t>
+  </si>
+  <si>
+    <t>AR(&lt;=2)</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,62 +1213,62 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
       <c r="K1" s="40"/>
       <c r="L1" s="41"/>
       <c r="M1" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="30" t="s">
+      <c r="H2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="M2" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,16 +1276,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>13</v>
@@ -1320,13 +1320,13 @@
         <v>20</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>11</v>
@@ -1355,13 +1355,13 @@
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>10</v>
@@ -1402,13 +1402,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>10</v>
@@ -1425,8 +1425,8 @@
       <c r="J6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>10</v>
+      <c r="K6" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>10</v>
@@ -1484,7 +1484,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
@@ -1519,13 +1519,13 @@
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="16" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>10</v>
@@ -1549,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L9" s="32" t="s">
         <v>10</v>
@@ -1566,7 +1566,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -1581,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>11</v>
@@ -1607,7 +1607,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>10</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>10</v>
@@ -1683,19 +1683,19 @@
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>10</v>
@@ -1724,13 +1724,13 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="C14" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>10</v>
@@ -1838,7 +1838,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,14 +1862,14 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
@@ -1877,34 +1877,34 @@
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="21"/>
     </row>
@@ -1913,7 +1913,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>11</v>
@@ -1937,7 +1937,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -1964,19 +1964,19 @@
         <v>11</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
@@ -2003,7 +2003,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K5" s="23"/>
     </row>
@@ -2108,10 +2108,10 @@
     </row>
     <row r="9" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>10</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="12" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="17" t="s">
@@ -2238,11 +2238,11 @@
     </row>
     <row r="13" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
@@ -2265,16 +2265,16 @@
         <v>10</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>51</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>52</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>10</v>
@@ -2363,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
@@ -2390,25 +2390,25 @@
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>11</v>
@@ -2431,7 +2431,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>11</v>
@@ -2457,7 +2457,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>10</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
@@ -2483,7 +2483,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>10</v>
@@ -2509,7 +2509,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>10</v>
@@ -2535,10 +2535,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2561,7 +2561,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>10</v>
@@ -2572,11 +2572,11 @@
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>10</v>
@@ -2613,7 +2613,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>10</v>
@@ -2639,7 +2639,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>10</v>
@@ -2650,11 +2650,11 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>10</v>
@@ -2676,11 +2676,11 @@
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>10</v>
@@ -2702,11 +2702,11 @@
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>52</v>
-      </c>
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>10</v>

</xml_diff>